<commit_message>
added data tokenizing function
</commit_message>
<xml_diff>
--- a/core/test_data/purchase_data_7Feb22.xlsx
+++ b/core/test_data/purchase_data_7Feb22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dudgk\Documents\GitHub\2022_kpmg_pinkcowlab\core\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83D044A-FB0E-41F0-9919-9FEBE49BA062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956FF4B5-7F63-4F0C-AE9F-D6F25C025533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="1440" windowWidth="19200" windowHeight="11360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="144">
   <si>
     <t>카카오페이지_카</t>
   </si>
@@ -109,9 +109,6 @@
     <t>(주)이니스프리제주하우스점</t>
   </si>
   <si>
-    <t>아모레퍼시픽</t>
-  </si>
-  <si>
     <t>씨유제주산방산점</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
   </si>
   <si>
     <t>카카오페이</t>
-  </si>
-  <si>
-    <t>지에스리테일(GS2</t>
   </si>
   <si>
     <t>연세대학교</t>
@@ -451,6 +445,18 @@
   </si>
   <si>
     <t>씨지브이대학로</t>
+  </si>
+  <si>
+    <t>이니스프리</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>지에스리테일(지에스2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>에뛰드하우스</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -736,8 +742,8 @@
   </sheetPr>
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -745,7 +751,7 @@
     <col min="1" max="1" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="14.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -754,7 +760,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="14.5">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -762,7 +768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="14.5">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -770,23 +776,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="14.5">
       <c r="A4" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.5">
+      <c r="A5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="14.5">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -794,7 +800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="14.5">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -802,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="14.5">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -810,7 +816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="14.5">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -818,23 +824,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="14.5">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.5">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.5">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -842,7 +848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="14.5">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -850,7 +856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="14.5">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -858,7 +864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="14.5">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -890,7 +896,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="14.5">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -898,7 +904,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="14.5">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -906,7 +912,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="14.5">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
@@ -919,132 +925,132 @@
         <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.5">
       <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.5">
+      <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.5">
       <c r="A25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="3" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="14.5">
+      <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.5">
+      <c r="A27" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" ht="14.5">
       <c r="A28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.5">
       <c r="A29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.5">
+      <c r="A30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.5">
+      <c r="A31" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" ht="14.5">
       <c r="A32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.5">
       <c r="A33" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.5">
       <c r="A34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="3" t="s">
+    </row>
+    <row r="35" spans="1:2" ht="14.5">
+      <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="B35" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.5">
       <c r="A36" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.5">
       <c r="A37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.5">
+      <c r="A38" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>9</v>
@@ -1052,15 +1058,15 @@
     </row>
     <row r="39" spans="1:2" ht="14.5">
       <c r="A39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.5">
+      <c r="A40" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>1</v>
@@ -1068,18 +1074,18 @@
     </row>
     <row r="41" spans="1:2" ht="14.5">
       <c r="A41" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="14.5">
+      <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="B42" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.5">
@@ -1092,23 +1098,23 @@
     </row>
     <row r="44" spans="1:2" ht="14.5">
       <c r="A44" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.5">
       <c r="A45" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.5">
       <c r="A46" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>17</v>
@@ -1116,39 +1122,39 @@
     </row>
     <row r="47" spans="1:2" ht="14.5">
       <c r="A47" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="14.5">
+      <c r="A48" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.5">
       <c r="A49" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="14.5">
+      <c r="A50" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B50" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.5">
+      <c r="A51" s="2" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>19</v>
@@ -1156,15 +1162,15 @@
     </row>
     <row r="52" spans="1:2" ht="14.5">
       <c r="A52" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.5">
       <c r="A53" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>1</v>
@@ -1172,39 +1178,39 @@
     </row>
     <row r="54" spans="1:2" ht="14.5">
       <c r="A54" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="14.5">
+      <c r="A55" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.5">
       <c r="A56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="14.5">
+      <c r="A57" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="B57" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.5">
       <c r="A58" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>25</v>
@@ -1212,39 +1218,39 @@
     </row>
     <row r="59" spans="1:2" ht="14.5">
       <c r="A59" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="14.5">
+      <c r="A60" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.5">
       <c r="A61" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.5">
+      <c r="A62" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="14.5">
+      <c r="A63" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>11</v>
@@ -1252,55 +1258,55 @@
     </row>
     <row r="64" spans="1:2" ht="14.5">
       <c r="A64" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="14.5">
+      <c r="A65" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="14.5">
+      <c r="A66" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="B66" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.5">
       <c r="A67" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="14.5">
       <c r="A68" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" ht="14.5">
       <c r="A69" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="14.5">
       <c r="A70" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>15</v>
@@ -1308,63 +1314,63 @@
     </row>
     <row r="71" spans="1:2" ht="14.5">
       <c r="A71" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.5">
       <c r="A72" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="14.5">
       <c r="A73" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="14.5">
       <c r="A74" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.5">
       <c r="A75" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="14.5">
       <c r="A76" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.5">
       <c r="A77" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="14.5">
       <c r="A78" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>17</v>
@@ -1372,23 +1378,23 @@
     </row>
     <row r="79" spans="1:2" ht="14.5">
       <c r="A79" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="14.5">
       <c r="A80" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="14.5">
       <c r="A81" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>1</v>
@@ -1396,95 +1402,95 @@
     </row>
     <row r="82" spans="1:2" ht="14.5">
       <c r="A82" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="14.5">
+      <c r="A83" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B83" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="14.5">
+      <c r="A84" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="B84" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.5">
       <c r="A85" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="14.5">
+      <c r="A86" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="14.5">
+      <c r="A87" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B85" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="2" t="s">
+      <c r="B87" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="14.5">
+      <c r="A88" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="B88" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.5">
       <c r="A89" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="14.5">
+      <c r="A90" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="14.5">
+      <c r="A91" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="2" t="s">
+      <c r="B91" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="2" t="s">
+    </row>
+    <row r="92" spans="1:2" ht="14.5">
+      <c r="A92" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B92" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="14.5">
+      <c r="A93" s="2" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>1</v>
@@ -1492,13 +1498,13 @@
     </row>
     <row r="94" spans="1:2" ht="14.5">
       <c r="A94" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="14.5">
       <c r="A95" s="2" t="s">
         <v>1</v>
       </c>
@@ -1508,47 +1514,47 @@
     </row>
     <row r="96" spans="1:2" ht="14.5">
       <c r="A96" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="14.5">
       <c r="A97" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" ht="14.5">
       <c r="A98" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="14.5">
+      <c r="A99" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="14.5">
+      <c r="A100" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B98" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="B100" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="14.5">
       <c r="A101" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>17</v>
@@ -1556,63 +1562,63 @@
     </row>
     <row r="102" spans="1:2" ht="14.5">
       <c r="A102" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="14.5">
+      <c r="A103" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="14.5">
       <c r="A104" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" ht="14.5">
       <c r="A105" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="14.5">
       <c r="A106" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" ht="14.5">
       <c r="A107" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="14.5">
+      <c r="A108" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B107" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="2" t="s">
+    </row>
+    <row r="109" spans="1:2" ht="14.5">
+      <c r="A109" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>1</v>

</xml_diff>